<commit_message>
Improve scraper for desired universities; dist and boxplots for EDA
</commit_message>
<xml_diff>
--- a/Data/Russian_Universities.xlsx
+++ b/Data/Russian_Universities.xlsx
@@ -205,25 +205,25 @@
     <t>56</t>
   </si>
   <si>
-    <t>E1</t>
-  </si>
-  <si>
-    <t>E2</t>
-  </si>
-  <si>
-    <t>E3</t>
-  </si>
-  <si>
-    <t>E4</t>
-  </si>
-  <si>
-    <t>E5</t>
-  </si>
-  <si>
-    <t>E6</t>
-  </si>
-  <si>
-    <t>E7</t>
+    <t>E.1</t>
+  </si>
+  <si>
+    <t>E.2</t>
+  </si>
+  <si>
+    <t>E.3</t>
+  </si>
+  <si>
+    <t>E.4</t>
+  </si>
+  <si>
+    <t>E.5</t>
+  </si>
+  <si>
+    <t>E.6</t>
+  </si>
+  <si>
+    <t>E.8</t>
   </si>
   <si>
     <t>MSU</t>

</xml_diff>

<commit_message>
Join all notebooks, universities time series
</commit_message>
<xml_diff>
--- a/Data/Russian_Universities.xlsx
+++ b/Data/Russian_Universities.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="231">
   <si>
     <t>University</t>
   </si>
@@ -706,58 +706,7 @@
     <t>Volgograd</t>
   </si>
   <si>
-    <t>201-250</t>
-  </si>
-  <si>
-    <t>1001+</t>
-  </si>
-  <si>
-    <t>801-1000</t>
-  </si>
-  <si>
-    <t>251-300</t>
-  </si>
-  <si>
-    <t>401-500</t>
-  </si>
-  <si>
-    <t>601-800</t>
-  </si>
-  <si>
-    <t>501-600</t>
-  </si>
-  <si>
-    <t>651-700</t>
-  </si>
-  <si>
-    <t>751-800</t>
-  </si>
-  <si>
-    <t>521-530</t>
-  </si>
-  <si>
-    <t>601-650</t>
-  </si>
-  <si>
-    <t>531-540</t>
-  </si>
-  <si>
-    <t>541-550</t>
-  </si>
-  <si>
-    <t>901-1000</t>
-  </si>
-  <si>
-    <t>601-700</t>
-  </si>
-  <si>
-    <t>301-400</t>
-  </si>
-  <si>
-    <t>801-900</t>
-  </si>
-  <si>
-    <t>701-800</t>
+    <t>1001</t>
   </si>
 </sst>
 </file>
@@ -1918,8 +1867,8 @@
       <c r="D3" t="s">
         <v>212</v>
       </c>
-      <c r="E3" t="s">
-        <v>230</v>
+      <c r="E3">
+        <v>242</v>
       </c>
       <c r="F3">
         <v>302</v>
@@ -1927,8 +1876,8 @@
       <c r="G3">
         <v>539</v>
       </c>
-      <c r="H3" t="s">
-        <v>234</v>
+      <c r="H3">
+        <v>499</v>
       </c>
       <c r="I3">
         <v>6483</v>
@@ -2311,10 +2260,10 @@
         <v>213</v>
       </c>
       <c r="E4" t="s">
-        <v>231</v>
-      </c>
-      <c r="F4" t="s">
-        <v>237</v>
+        <v>230</v>
+      </c>
+      <c r="F4">
+        <v>669</v>
       </c>
       <c r="I4">
         <v>14283</v>
@@ -2696,8 +2645,8 @@
       <c r="D5" t="s">
         <v>212</v>
       </c>
-      <c r="E5" t="s">
-        <v>232</v>
+      <c r="E5">
+        <v>983</v>
       </c>
       <c r="F5">
         <v>284</v>
@@ -3082,8 +3031,8 @@
       <c r="D6" t="s">
         <v>212</v>
       </c>
-      <c r="E6" t="s">
-        <v>233</v>
+      <c r="E6">
+        <v>278</v>
       </c>
       <c r="F6">
         <v>322</v>
@@ -3091,8 +3040,8 @@
       <c r="G6">
         <v>879</v>
       </c>
-      <c r="H6" t="s">
-        <v>243</v>
+      <c r="H6">
+        <v>983</v>
       </c>
       <c r="I6">
         <v>28755</v>
@@ -3474,8 +3423,8 @@
       <c r="D7" t="s">
         <v>212</v>
       </c>
-      <c r="E7" t="s">
-        <v>234</v>
+      <c r="E7">
+        <v>437</v>
       </c>
       <c r="F7">
         <v>329</v>
@@ -3483,8 +3432,8 @@
       <c r="G7">
         <v>726</v>
       </c>
-      <c r="H7" t="s">
-        <v>244</v>
+      <c r="H7">
+        <v>638</v>
       </c>
       <c r="I7">
         <v>5586</v>
@@ -4249,8 +4198,8 @@
       <c r="D9" t="s">
         <v>212</v>
       </c>
-      <c r="E9" t="s">
-        <v>232</v>
+      <c r="E9">
+        <v>953</v>
       </c>
       <c r="F9">
         <v>392</v>
@@ -4638,8 +4587,8 @@
       <c r="D10" t="s">
         <v>212</v>
       </c>
-      <c r="E10" t="s">
-        <v>235</v>
+      <c r="E10">
+        <v>682</v>
       </c>
       <c r="F10">
         <v>451</v>
@@ -5027,8 +4976,8 @@
       <c r="D11" t="s">
         <v>212</v>
       </c>
-      <c r="F11" t="s">
-        <v>238</v>
+      <c r="F11">
+        <v>792</v>
       </c>
       <c r="I11">
         <v>17787</v>
@@ -5410,8 +5359,8 @@
       <c r="D12" t="s">
         <v>214</v>
       </c>
-      <c r="E12" t="s">
-        <v>235</v>
+      <c r="E12">
+        <v>644</v>
       </c>
       <c r="F12">
         <v>234</v>
@@ -5419,8 +5368,8 @@
       <c r="G12">
         <v>560</v>
       </c>
-      <c r="H12" t="s">
-        <v>245</v>
+      <c r="H12">
+        <v>316</v>
       </c>
       <c r="I12">
         <v>19277</v>
@@ -5802,8 +5751,8 @@
       <c r="D13" t="s">
         <v>214</v>
       </c>
-      <c r="E13" t="s">
-        <v>234</v>
+      <c r="E13">
+        <v>447</v>
       </c>
       <c r="F13">
         <v>436</v>
@@ -5811,8 +5760,8 @@
       <c r="G13">
         <v>1002</v>
       </c>
-      <c r="H13" t="s">
-        <v>246</v>
+      <c r="H13">
+        <v>853</v>
       </c>
       <c r="I13">
         <v>12127</v>
@@ -6194,8 +6143,8 @@
       <c r="D14" t="s">
         <v>214</v>
       </c>
-      <c r="E14" t="s">
-        <v>236</v>
+      <c r="E14">
+        <v>521</v>
       </c>
       <c r="F14">
         <v>439</v>
@@ -6584,10 +6533,10 @@
         <v>215</v>
       </c>
       <c r="E15" t="s">
-        <v>231</v>
-      </c>
-      <c r="F15" t="s">
-        <v>232</v>
+        <v>230</v>
+      </c>
+      <c r="F15">
+        <v>809</v>
       </c>
       <c r="I15">
         <v>17135</v>
@@ -6969,8 +6918,8 @@
       <c r="D16" t="s">
         <v>216</v>
       </c>
-      <c r="E16" t="s">
-        <v>236</v>
+      <c r="E16">
+        <v>594</v>
       </c>
       <c r="F16">
         <v>268</v>
@@ -6978,8 +6927,8 @@
       <c r="G16">
         <v>983</v>
       </c>
-      <c r="H16" t="s">
-        <v>246</v>
+      <c r="H16">
+        <v>842</v>
       </c>
       <c r="I16">
         <v>13578</v>
@@ -7361,8 +7310,8 @@
       <c r="D17" t="s">
         <v>216</v>
       </c>
-      <c r="E17" t="s">
-        <v>235</v>
+      <c r="E17">
+        <v>640</v>
       </c>
       <c r="F17">
         <v>387</v>
@@ -7370,8 +7319,8 @@
       <c r="G17">
         <v>1399</v>
       </c>
-      <c r="H17" t="s">
-        <v>246</v>
+      <c r="H17">
+        <v>847</v>
       </c>
       <c r="I17">
         <v>11720</v>
@@ -7753,8 +7702,8 @@
       <c r="D18" t="s">
         <v>217</v>
       </c>
-      <c r="E18" t="s">
-        <v>236</v>
+      <c r="E18">
+        <v>542</v>
       </c>
       <c r="F18">
         <v>231</v>
@@ -7762,8 +7711,8 @@
       <c r="G18">
         <v>610</v>
       </c>
-      <c r="H18" t="s">
-        <v>234</v>
+      <c r="H18">
+        <v>449</v>
       </c>
       <c r="I18">
         <v>7690</v>
@@ -8146,10 +8095,10 @@
         <v>217</v>
       </c>
       <c r="E19" t="s">
-        <v>231</v>
-      </c>
-      <c r="F19" t="s">
-        <v>232</v>
+        <v>230</v>
+      </c>
+      <c r="F19">
+        <v>929</v>
       </c>
       <c r="I19">
         <v>13234</v>
@@ -8532,10 +8481,10 @@
         <v>218</v>
       </c>
       <c r="E20" t="s">
-        <v>231</v>
-      </c>
-      <c r="F20" t="s">
-        <v>239</v>
+        <v>230</v>
+      </c>
+      <c r="F20">
+        <v>529</v>
       </c>
       <c r="I20">
         <v>17897</v>
@@ -8917,8 +8866,8 @@
       <c r="D21" t="s">
         <v>219</v>
       </c>
-      <c r="E21" t="s">
-        <v>235</v>
+      <c r="E21">
+        <v>601</v>
       </c>
       <c r="F21">
         <v>392</v>
@@ -8926,8 +8875,8 @@
       <c r="G21">
         <v>1090</v>
       </c>
-      <c r="H21" t="s">
-        <v>246</v>
+      <c r="H21">
+        <v>860</v>
       </c>
       <c r="I21">
         <v>32358</v>
@@ -9310,10 +9259,10 @@
         <v>220</v>
       </c>
       <c r="E22" t="s">
-        <v>231</v>
-      </c>
-      <c r="F22" t="s">
-        <v>240</v>
+        <v>230</v>
+      </c>
+      <c r="F22">
+        <v>607</v>
       </c>
       <c r="G22">
         <v>1505</v>
@@ -9699,7 +9648,7 @@
         <v>221</v>
       </c>
       <c r="E23" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F23">
         <v>364</v>
@@ -9707,8 +9656,8 @@
       <c r="G23">
         <v>1198</v>
       </c>
-      <c r="H23" t="s">
-        <v>247</v>
+      <c r="H23">
+        <v>703</v>
       </c>
       <c r="I23">
         <v>33458</v>
@@ -10091,10 +10040,10 @@
         <v>222</v>
       </c>
       <c r="E24" t="s">
-        <v>231</v>
-      </c>
-      <c r="F24" t="s">
-        <v>241</v>
+        <v>230</v>
+      </c>
+      <c r="F24">
+        <v>535</v>
       </c>
       <c r="G24">
         <v>1804</v>
@@ -10480,10 +10429,10 @@
         <v>223</v>
       </c>
       <c r="E25" t="s">
-        <v>231</v>
-      </c>
-      <c r="F25" t="s">
-        <v>232</v>
+        <v>230</v>
+      </c>
+      <c r="F25">
+        <v>914</v>
       </c>
       <c r="I25">
         <v>24762</v>
@@ -10866,10 +10815,10 @@
         <v>224</v>
       </c>
       <c r="E26" t="s">
-        <v>231</v>
-      </c>
-      <c r="F26" t="s">
-        <v>242</v>
+        <v>230</v>
+      </c>
+      <c r="F26">
+        <v>547</v>
       </c>
       <c r="G26">
         <v>1489</v>
@@ -11254,8 +11203,8 @@
       <c r="D27" t="s">
         <v>214</v>
       </c>
-      <c r="E27" t="s">
-        <v>232</v>
+      <c r="E27">
+        <v>922</v>
       </c>
       <c r="I27">
         <v>7705</v>
@@ -11638,7 +11587,7 @@
         <v>225</v>
       </c>
       <c r="E28" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I28">
         <v>14804</v>
@@ -12021,7 +11970,7 @@
         <v>226</v>
       </c>
       <c r="E29" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I29">
         <v>16395</v>
@@ -12404,7 +12353,7 @@
         <v>212</v>
       </c>
       <c r="E30" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I30">
         <v>9204</v>
@@ -12787,7 +12736,7 @@
         <v>212</v>
       </c>
       <c r="E31" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I31">
         <v>24807</v>
@@ -13170,7 +13119,7 @@
         <v>212</v>
       </c>
       <c r="E32" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I32">
         <v>18959</v>
@@ -13553,7 +13502,7 @@
         <v>212</v>
       </c>
       <c r="E33" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I33">
         <v>14069</v>
@@ -13936,7 +13885,7 @@
         <v>227</v>
       </c>
       <c r="E34" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I34">
         <v>13587</v>
@@ -14319,7 +14268,7 @@
         <v>227</v>
       </c>
       <c r="E35" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I35">
         <v>12075</v>
@@ -14702,7 +14651,7 @@
         <v>212</v>
       </c>
       <c r="E36" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I36">
         <v>8225</v>
@@ -15085,7 +15034,7 @@
         <v>212</v>
       </c>
       <c r="E37" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I37">
         <v>15903</v>
@@ -15468,7 +15417,7 @@
         <v>228</v>
       </c>
       <c r="E38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G38">
         <v>1859</v>
@@ -15854,7 +15803,7 @@
         <v>214</v>
       </c>
       <c r="E39" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I39">
         <v>8996</v>
@@ -16237,7 +16186,7 @@
         <v>225</v>
       </c>
       <c r="E40" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I40">
         <v>13035</v>
@@ -16620,7 +16569,7 @@
         <v>229</v>
       </c>
       <c r="E41" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I41">
         <v>14043</v>
@@ -17003,7 +16952,7 @@
         <v>212</v>
       </c>
       <c r="E42" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I42">
         <v>610</v>

</xml_diff>